<commit_message>
Add startGame, startRound, getGameState API
</commit_message>
<xml_diff>
--- a/doc/flow.xlsx
+++ b/doc/flow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\liar\LiarGameServer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7048A3B8-E4CF-457B-B2C9-0DCDE66EAFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6FD42BA-9DF8-4F71-91D0-9CA77313368F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="153">
   <si>
     <t>단계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -562,33 +562,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>/publish.system.room.{roomId} 또는 /publish.system.room.{roomId}/API</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>파라미터 예시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"method":"startGame", "body":{"round":8,"category":{"food"]}},"turn":2})}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>round:int,
-category:list&lt;string&gt;,
-turn:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>REQUEST_LIAR_ANSWER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>state:"before_round"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>state:"select_liar",round:int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -635,6 +613,99 @@
   </si>
   <si>
     <t>turn:[string]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*spring state machine 분석
+*chattingcontroller test 코드구현
+*gameContoller startGame test 코드 구현중</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*gameContoller startGame/startRound/selectLiar test 코드 구현예정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>senderId:String
+message:{
+            "method":String
+            "body":JSON.stringify
+            (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>round:int,
+            category:list&lt;string&gt;,
+            turn:int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+        },
+"uuid":String</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"senderId":125414y71hf21,
+        "message":{
+            "method":"startGame",
+            "body":
+JSON.stringify({"round":3,
+                "category":["food"],
+                "turn":1
+            })
+        },
+"uuid":1231125ds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>"senderId":"SERVER",
+        "message":{
+            "method":"notifyGameStarted",
+            "body":
+JSON.stringify({"state":"BEFORE_ROUND"})
+},
+"uuid":1231125ds</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state:"BEFORE_ROUND"</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/publish/system/private/{roomId} 또는 /publish/system/public/{roomId}/API</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER",
+"message":
+{
+"method":"notifyRoundStarted",
+"body":{
+"state":"SELECT_LIAR",
+"round":1}"},
+"uuid":"237f5643-bfd7-e6d6-59dd-96a537006e4a"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>state:"SELECT_LIAR",round:int</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -645,7 +716,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -672,6 +743,15 @@
     </font>
     <font>
       <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="맑은 고딕"/>
@@ -742,11 +822,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1064,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1073,20 +1153,21 @@
     <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.125" customWidth="1"/>
-    <col min="6" max="7" width="30.25" style="3" customWidth="1"/>
+    <col min="5" max="5" width="33.875" customWidth="1"/>
+    <col min="6" max="6" width="30.25" style="3" customWidth="1"/>
+    <col min="7" max="7" width="33.625" style="3" customWidth="1"/>
     <col min="8" max="8" width="44.375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="40.25" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.25" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="66" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
       <c r="E1" s="6" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="F1" s="6"/>
       <c r="G1" s="6"/>
@@ -1116,7 +1197,7 @@
         <v>65</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>5</v>
@@ -1144,8 +1225,8 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:10" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
       <c r="B4" s="5">
@@ -1161,10 +1242,10 @@
         <v>62</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>134</v>
+        <v>146</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>12</v>
@@ -1172,8 +1253,8 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
@@ -1187,9 +1268,11 @@
         <v>87</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G5" s="6"/>
+        <v>149</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>148</v>
+      </c>
       <c r="H5" s="6" t="s">
         <v>13</v>
       </c>
@@ -1201,7 +1284,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="13"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="5" t="s">
         <v>76</v>
       </c>
@@ -1225,7 +1308,7 @@
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="13"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="5" t="s">
         <v>77</v>
       </c>
@@ -1249,7 +1332,7 @@
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="13"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="1" t="s">
         <v>110</v>
       </c>
@@ -1271,7 +1354,7 @@
       <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="1" t="s">
         <v>114</v>
       </c>
@@ -1291,7 +1374,7 @@
       <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="14" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1307,7 +1390,7 @@
         <v>67</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6" t="s">
@@ -1316,8 +1399,8 @@
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
     </row>
-    <row r="11" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
+    <row r="11" spans="1:10" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1331,9 +1414,11 @@
         <v>88</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="G11" s="6"/>
+        <v>152</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>151</v>
+      </c>
       <c r="H11" s="6" t="s">
         <v>15</v>
       </c>
@@ -1343,7 +1428,7 @@
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="14" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -1359,7 +1444,7 @@
         <v>69</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6" t="s">
@@ -1369,7 +1454,7 @@
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
@@ -1383,10 +1468,10 @@
         <v>89</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>19</v>
@@ -1399,7 +1484,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="14" t="s">
         <v>54</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -1412,10 +1497,10 @@
         <v>11</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="G14" s="6"/>
       <c r="H14" s="6" t="s">
@@ -1427,21 +1512,21 @@
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="5" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>90</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
@@ -1449,7 +1534,7 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A16" s="13"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="5" t="s">
         <v>85</v>
       </c>
@@ -1463,7 +1548,7 @@
         <v>93</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6" t="s">
@@ -1477,7 +1562,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -1503,7 +1588,7 @@
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" ht="132" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="5"/>
       <c r="C18" s="9" t="s">
         <v>4</v>
@@ -1529,7 +1614,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="5"/>
       <c r="C19" s="9" t="s">
         <v>4</v>
@@ -1551,7 +1636,7 @@
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="5"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -1563,7 +1648,7 @@
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="5"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1575,7 +1660,7 @@
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="14" t="s">
         <v>60</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -1600,7 +1685,7 @@
       <c r="J22" s="6"/>
     </row>
     <row r="23" spans="1:10" ht="66" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="5" t="s">
         <v>23</v>
       </c>
@@ -1626,7 +1711,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="13"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="5" t="s">
         <v>25</v>
       </c>
@@ -1648,7 +1733,7 @@
       <c r="J24" s="6"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="13"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="5" t="s">
         <v>101</v>
       </c>
@@ -1670,7 +1755,7 @@
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="14" t="s">
         <v>55</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -1694,7 +1779,7 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="13"/>
+      <c r="A27" s="14"/>
       <c r="B27" s="5" t="s">
         <v>29</v>
       </c>
@@ -1716,7 +1801,7 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="33" x14ac:dyDescent="0.3">
-      <c r="A28" s="13"/>
+      <c r="A28" s="14"/>
       <c r="B28" s="5" t="s">
         <v>28</v>
       </c>
@@ -1742,8 +1827,8 @@
       <c r="J28" s="6"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
-        <v>135</v>
+      <c r="A29" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>33</v>
@@ -1766,7 +1851,7 @@
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="1:10" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="13"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="5" t="s">
         <v>32</v>
       </c>
@@ -1792,7 +1877,7 @@
       <c r="J30" s="6"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="14" t="s">
         <v>57</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -1814,7 +1899,7 @@
       <c r="J31" s="6"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="13"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="5" t="s">
         <v>39</v>
       </c>
@@ -1963,10 +2048,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0688698-043E-4F34-83E0-0B082EC495A7}">
-  <dimension ref="B1:C2"/>
+  <dimension ref="B1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1977,15 +2062,31 @@
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="2:3" ht="66" x14ac:dyDescent="0.3">
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>44898</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>147</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="66" x14ac:dyDescent="0.3">
+      <c r="B3" s="13">
+        <v>44899</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="13">
+        <v>44900</v>
+      </c>
+      <c r="C4" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[ADD] OPEN_LIAR/LIAR_ANSWER /PUBLISH_SCORE state service && controller code implementation
</commit_message>
<xml_diff>
--- a/doc/flow.xlsx
+++ b/doc/flow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\liar\LiarGameServer\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA67A81-7C57-480A-8FAC-80359F1F2931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7183252C-342D-46F6-B57B-BE028940157C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4615DC25-7943-4644-A7C8-5BBD0D70B551}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="188">
   <si>
     <t>단계</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -147,10 +147,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5-1-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>6-1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,10 +175,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>라이어에게 정답 말하라고함</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>정답 공개</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -191,22 +183,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>정답 확인 요청</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>7-1-2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>라이어의 정답여부 알림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>7-1-3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>점수 공개</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -231,14 +211,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>8-1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>순위 공개</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BEFORE_ROUND</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -255,17 +227,9 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>OPEN_LIAR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>END_ROUND</t>
   </si>
   <si>
-    <t>CHECK_LIAR_ANSWER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PUBLISH_SCORE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -350,10 +314,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>라이어공개 요청하라고 알림&lt;-필요할까?</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>notifyGameStarted</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -422,10 +382,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>notifyLiarOpenNeeded</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>notifyLiarOpened</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -466,34 +422,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>state,clientId(liar)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>state,answer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>notifyLiarAnswerCorrect</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>isCorrectAnswer</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>현재 state확인. 요청자가 라이어가 맞는지확인. RoundController에게 정답여부 요청. check_liar_answer state로 변경</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>answer:yes/no</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[clientid:점수]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>RoundController에 점수계산요청</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -506,19 +442,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>7-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>파라미터 예시</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>REQUEST_LIAR_ANSWER</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>null</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -569,43 +493,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>"senderId":125414y71hf21,
-        "message":{
-            "method":"startGame",
-            "body":
-JSON.stringify({"round":3,
-                "category":["food"],
-                "turn":1
-            })
-        },
-"uuid":1231125ds</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>state:"BEFORE_ROUND"</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"senderId":"SERVER",
-"message":
-{
-"method":"notifyRoundStarted",
-"body":{
-"state":"SELECT_LIAR",
-"round":1}"},
-"uuid":"237f5643-bfd7-e6d6-59dd-96a537006e4a"}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>state:"SELECT_LIAR",round:int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"liar":true(라이어일경우)}
-{"liar":false(라이어가아닐경우)}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>*gameContoller startGame/startRound/selectLiar test 코드 구현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -672,11 +559,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"senderId":"SERVER",
-"message":{"method":"notifyKeywordOpened", "body":{"category":"sports","keyword":"soccer","turnOrder":["8b3ba077-cc04-4702-b6ae-15a630fb0df6","d937f134-c43d-44ed-bfd1-9f07f719690c"],"state":"IN_PROGRESS"}}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -708,16 +590,6 @@
   </si>
   <si>
     <t>requestTurnFinish</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"senderId":"SERVER",
-"message":
-{
-"method":"notifyRoundEnd",
-"body":{
-"state":"VOTE_LIAR",
-"round":1}"}}</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -806,10 +678,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>{"senderId":"SERVER", "message":{"method":"notifyGameStarted", "body":{"state":"BEFORE_ROUND"}}}, "uuid":'65c1c59f-4c03-489f-8692-5483d429caa2'}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>구현완료된 API 표시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -889,30 +757,1163 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>state:String
-round:Int</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"liar":String</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>"voteResult":Map&lt;String,int&gt;
-"MostVoted":List&lt;Pair&lt;String,Int&gt;&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{"senderId":"SERVER",
-"message":
-{
-"method":"notifyNewVoteNeeded",
-"body":{
-"state":"VOTE_LIAR"}"}}</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>*voteLiar API 구현 및 테스트코드 구현</t>
+    <t>checkKeywordCorrect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LIAR_ANSWER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">타임아웃에 따라 라이어의 정답여부 알림
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/publish/system/private/{roomId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"startGame", "body":{"round":5,"turn":2,"category":["food","sports"]}}, "uuid":"a8f5bdc9-3cc7-4d9f-bde5-71ef471b9308"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyGameStarted", "body":{"state":"BEFORE_ROUND"}}, "uuid":"a8f5bdc9-3cc7-4d9f-bde5-71ef471b9308"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"startRound", "body":{}}, "uuid":"7d9fd1d0-078d-443b-85cd-249b2ac021f2"}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>senderId:String
+message:{
+            "method":String
+            "body":JSON.stringify
+            (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>state:String</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+        },
+"uuid":String</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>senderId:String
+message:{
+            "method":String
+            "body":JSON.stringify
+            (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"{}"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+        },
+"uuid":String</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":
+{"method":"notifyRoundStarted", "body":
+JSON.stringify({</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"state":"SELECT_LIAR","round":int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>})
+}, "uuid":String}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>openKeyword</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{}}, "uuid":"6c9bfe42-4a37-4ede-a7a8-76ecd80c958a"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyLiarSelected</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"liar":true/false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"state":"OPEN_KEYWORD"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":'dcd4e79d-8908-4e3c-968b-b5b9addccf16'}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>selectLiar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{}}, "uuid":"dcd4e79d-8908-4e3c-968b-b5b9addccf16"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyRoundStarted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"state":"SELECT_LIAR","round":1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":"7d9fd1d0-078d-443b-85cd-249b2ac021f2"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyTurn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"turnId":"2c1c2918-98ba-4360-af3f-61984ebcc924",
+"state":"IN_PROGRESS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":"b4937351-7a09-4488-91b7-3d8b529cf5d6"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyKeywordOpened</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">", "body":{
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"category":"sports",
+"keyword":"LIAR",
+"turnOrder":["2c1c2918-98ba-4360-af3f-61984ebcc924","1b60ce03-8aba-48e5-82a9-dec28c03e6c6"],
+"state":"IN_PROGRESS"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":"6c9bfe42-4a37-4ede-a7a8-76ecd80c958a"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>requestTurnFinished</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{}}, "uuid":"f8542777-28de-4a11-ab30-ed45ba4bf762"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyRoundEnd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"state":"VOTE_LIAR","round":2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":"5c91a9a9-f6d9-42d9-8452-394c71f42589"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"2c1c2918-98ba-4360-af3f-61984ebcc924", "message":{"method":"voteLiar", "body":{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"liar":"1b60ce03-8aba-48e5-82a9-dec28c03e6c6"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":"dab3c087-0a7d-4029-8e5b-72b14fbdc695"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyVoteResult</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">", "body":{
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"voteResult":{"1b60ce03-8aba-48e5-82a9-dec28c03e6c6":"1b60ce03-8aba-48e5-82a9-dec28c03e6c6","2c1c2918-98ba-4360-af3f-61984ebcc924":"1b60ce03-8aba-48e5-82a9-dec28c03e6c6"},
+"mostVoted":[{"1b60ce03-8aba-48e5-82a9-dec28c03e6c6":2}]}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}, "uuid":'02c2fccd-f151-462f-b41b-b233da62cd22'}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":String, "message":{"method":"openLiar", "body":{}}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"2f76478e-163c-4df5-a158-de39f02c9fef", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>openLiar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{}}, "uuid":'a97103ee-f9d6-429f-9723-35486b4e3731'}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyLiarOpened", "body":{
+"liar":String,
+"state":"LIAR_ANSWER","matchLiar":boolean}}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER",
+"message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyLiarOpened</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{"liar":"698087f6-3847-4898-b119-993681ad450a","state":"LIAR_ANSWER","matchLiar":true/false</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":"701cfae6-f879-4de0-804c-390fa1842627"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{"senderId":"SERVER", "message":{"method":"notifyRoundEnd", "body":{
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"state":"VOTE_LIAR",
+"round":int</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":String}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">{"senderId":String, "message":{
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"method":"voteLiar", "body":{"liar":String}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}, "uuid":String}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"notifyVoteResult", "body":</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{"voteResult":List&lt;String,String&gt;,
+"mostVoted":List&lt;String,int&gt;}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}, "uuid":String}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyNewVoteNeeded</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"state":"VOTE_LIAR"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":"80952c25-a046-4e6c-8519-1b4bae0ea86b"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{
+"method":"notifyNewVoteNeeded", "body":{"state":"VOTE_LIAR"}}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":
+{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyTurnTimeout</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{}}, "uuid":"8044cf67-0083-4fa4-acbd-ef40788a6057"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyLiarAnswerNeeded</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{}}, "uuid":"89e48c7e-fbb2-4b94-b9ae-022890deff7f"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"notifyLiarAnswerNeeded", "body":</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}, "uuid":String}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"String, "message":{"method":"checkKeywordCorrect", 
+"body":{"keyword":String}}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"16020f2d-5a86-4fdb-88a1-3a377d25d87a", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>checkKeywordCorrect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{"keyword":"keyword"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":'07a0e776-601c-49b4-a005-118e322c2838'}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notifyLiarAnswerTimeout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>openScores</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>/subscribe/system/private/{liarId}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>라이어에게 정답 reply 요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10-1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":String, "message":{"method":"openScore", "body":{}}, 
+"uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyScores", "body":{"scoreBoard":Map&lt;String,int&gt;}}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"85b753c2-90cf-4522-a7af-d900b41b2711", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>openScore</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{}}, "uuid":"59d33d69-5270-44ec-9d94-4ede767a5161"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyScores</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{"scoreBoard":{"85b753c2-90cf-4522-a7af-d900b41b2711":3,"7a7ba6e6-3c67-4d7c-8d1a-b8d0a18c961a":0}}}, "uuid":'82cd0ea6-f181-4e01-ba25-85465555c655'}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*OPEN_LIAR/LIAR_ANSWER /PUBLISH_SCORE controller 코드 및 테스트코드 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*voteLiar API 구현 및 테스트코드 구현
+*OPEN_LIAR/LIAR_ANSWER /PUBLISH_SCORE service 및 테스트코드 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>남은일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정답 공개 확인 요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>{"senderId":"SERVER", "message":{"method":"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>notifyLiarAnswerCorrect</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>", "body":{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"answer":true/false,"state":"PUBLISH_SCORE"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}}, "uuid":"7684edb2-0e6b-48fc-880c-39b09d73f3d3"}</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{"senderId":"SERVER", "message":{"method":"notifyLiarAnswerCorrect", "body":{"answer":boolean,"state":"PUBLISH_SCORE"}}, "uuid":String}</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>*타임아웃관련 API
+*라운드처리
+*랭킹 처리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체순위 공개</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전체순위 공개 요청</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -936,24 +1937,6 @@
       <sz val="8"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="맑은 고딕"/>
-      <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
@@ -985,6 +1968,23 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -1032,11 +2032,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1058,13 +2058,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1073,23 +2073,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1406,22 +2403,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C429DD-F26C-4C33-AAA9-E705D35C568E}">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.875" customWidth="1"/>
-    <col min="7" max="7" width="34.25" style="3" customWidth="1"/>
-    <col min="8" max="8" width="33.625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="44.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="44.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.875" customWidth="1"/>
+    <col min="8" max="8" width="36" style="3" customWidth="1"/>
+    <col min="9" max="9" width="33.625" style="3" customWidth="1"/>
     <col min="10" max="10" width="40.25" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.25" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -1429,13 +2426,13 @@
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="5"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="5"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
-      <c r="F1" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="8"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="7" t="s">
+        <v>116</v>
+      </c>
       <c r="H1" s="8"/>
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
@@ -1444,13 +2441,13 @@
     <row r="2" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="6"/>
-      <c r="C2" s="5"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="G2" s="8"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="9" t="s">
+        <v>110</v>
+      </c>
       <c r="H2" s="8"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8" t="s">
@@ -1460,31 +2457,31 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>144</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>64</v>
+        <v>117</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>118</v>
+        <v>55</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="J3" s="11" t="s">
         <v>7</v>
@@ -1495,865 +2492,932 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="C4" s="8"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="8"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
       <c r="K4" s="8"/>
     </row>
-    <row r="5" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
-        <v>46</v>
+    <row r="5" spans="1:11" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="14" t="s">
+        <v>41</v>
       </c>
       <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>123</v>
+      <c r="F5" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>52</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>12</v>
+        <v>139</v>
       </c>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="14"/>
       <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>125</v>
+      <c r="F6" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>69</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>142</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>13</v>
+        <v>140</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>155</v>
+        <v>128</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>73</v>
+        <v>62</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8" t="s">
-        <v>75</v>
-      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="8"/>
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8" t="s">
-        <v>99</v>
-      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="8"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>73</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="C9" s="8"/>
       <c r="D9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H9" s="8"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>89</v>
+      </c>
       <c r="I9" s="8"/>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="E10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="H10" s="8"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>74</v>
+      </c>
       <c r="I10" s="8"/>
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>50</v>
+    <row r="11" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="14" t="s">
+        <v>43</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="E11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="H11" s="8"/>
+      <c r="F11" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="I11" s="8" t="s">
-        <v>69</v>
+        <v>141</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="17"/>
+    <row r="12" spans="1:11" ht="99" x14ac:dyDescent="0.3">
+      <c r="A12" s="14"/>
       <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="J12" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="H12" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="8" t="s">
-        <v>154</v>
-      </c>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="17" t="s">
-        <v>51</v>
+    <row r="13" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="14" t="s">
+        <v>44</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
+      <c r="F13" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="I13" s="8" t="s">
-        <v>17</v>
+        <v>147</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="F14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H14" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>19</v>
-      </c>
       <c r="J14" s="8" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="17" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="E15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="F15" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I15" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8" t="s">
-        <v>132</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="17"/>
+    <row r="16" spans="1:11" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="14"/>
       <c r="B16" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C16" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>133</v>
+      <c r="F16" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>72</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>52</v>
+        <v>109</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>150</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>152</v>
+        <v>125</v>
       </c>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="17" t="s">
-        <v>47</v>
+    <row r="17" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="E17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="F17" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8" t="s">
-        <v>86</v>
+      <c r="G17" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>164</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" ht="132" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="J18" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="J18" s="8" t="s">
-        <v>93</v>
-      </c>
       <c r="K18" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="14"/>
       <c r="B19" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>73</v>
+        <v>79</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>122</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>137</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="H19" s="8"/>
+      <c r="F19" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="I19" s="8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="17"/>
+    <row r="20" spans="1:11" ht="99" x14ac:dyDescent="0.3">
+      <c r="A20" s="14"/>
       <c r="B20" s="6"/>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>160</v>
+      <c r="F20" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>77</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>88</v>
+        <v>152</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>156</v>
+        <v>129</v>
       </c>
       <c r="K20" s="8"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="17" t="s">
-        <v>59</v>
+    <row r="21" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A21" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="H21" s="8"/>
+      <c r="F21" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="I21" s="8" t="s">
-        <v>22</v>
+        <v>153</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
+    <row r="22" spans="1:11" ht="231" x14ac:dyDescent="0.3">
+      <c r="A22" s="14"/>
       <c r="B22" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="H22" s="8"/>
+      <c r="F22" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>161</v>
+      </c>
       <c r="I22" s="8" t="s">
-        <v>24</v>
+        <v>154</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="99" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+      <c r="A23" s="14"/>
       <c r="B23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8" t="s">
+      <c r="F23" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H23" s="9" t="s">
         <v>163</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>26</v>
+        <v>162</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="C24" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="E24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="G24" s="8"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5" t="s">
+        <v>81</v>
+      </c>
       <c r="H24" s="8"/>
-      <c r="I24" s="8" t="s">
-        <v>90</v>
-      </c>
+      <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="17" t="s">
-        <v>54</v>
-      </c>
+    <row r="25" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A25" s="14"/>
       <c r="B25" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+        <v>138</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>155</v>
+      </c>
       <c r="I25" s="8" t="s">
-        <v>78</v>
+        <v>156</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="17"/>
+    <row r="26" spans="1:11" ht="132" x14ac:dyDescent="0.3">
+      <c r="A26" s="14"/>
       <c r="B26" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>3</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>145</v>
+        <v>11</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+        <v>119</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>157</v>
+      </c>
       <c r="I26" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="J26" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A27" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="1:11" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="A28" s="14"/>
+      <c r="B28" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="A27" s="17"/>
-      <c r="B27" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="5" t="s">
+      <c r="C28" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="F28" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>133</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="J28" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:11" ht="99" x14ac:dyDescent="0.3">
+      <c r="A29" s="14"/>
+      <c r="B29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="K27" s="8"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="17" t="s">
+      <c r="F29" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A30" s="14"/>
+      <c r="B30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="5" t="s">
+      <c r="G30" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="17"/>
-      <c r="B29" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="5" t="s">
+      <c r="F31" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" ht="132" x14ac:dyDescent="0.3">
+      <c r="A32" s="14"/>
+      <c r="B32" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J29" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="K29" s="8"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="17"/>
-      <c r="B31" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="J31" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="K31" s="8"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="5"/>
       <c r="F32" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G32" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="H32" s="8"/>
+        <v>119</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>176</v>
+      </c>
       <c r="I32" s="8" t="s">
-        <v>42</v>
+        <v>178</v>
       </c>
       <c r="J32" s="8"/>
       <c r="K32" s="8"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="10"/>
+      <c r="A33" s="10" t="s">
+        <v>47</v>
+      </c>
       <c r="B33" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>3</v>
+        <v>136</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>4</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="8"/>
+        <v>11</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G33" s="5"/>
       <c r="H33" s="8"/>
-      <c r="I33" s="8" t="s">
-        <v>116</v>
-      </c>
+      <c r="I33" s="8"/>
       <c r="J33" s="8"/>
       <c r="K33" s="8"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C34" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="D34" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="8"/>
+      <c r="F34" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G34" s="5"/>
       <c r="H34" s="8"/>
-      <c r="I34" s="8" t="s">
-        <v>44</v>
-      </c>
+      <c r="I34" s="8"/>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="I36" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
+      <c r="A36" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A32"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A21:A24"/>
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A25:A27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2362,85 +3426,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0688698-043E-4F34-83E0-0B082EC495A7}">
-  <dimension ref="B1:C9"/>
+  <dimension ref="B1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="59.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.25" customWidth="1"/>
+    <col min="6" max="6" width="9.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" ht="49.5" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="2:6" ht="99" x14ac:dyDescent="0.3">
       <c r="B2" s="4">
         <v>44898</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="49.5" x14ac:dyDescent="0.3">
+        <v>106</v>
+      </c>
+      <c r="E2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>44899</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>44900</v>
       </c>
       <c r="C4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="4">
         <v>44902</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="33" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="33" x14ac:dyDescent="0.3">
       <c r="B6" s="4">
         <v>44906</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>44908</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>44909</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>44913</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>164</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>44914</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>